<commit_message>
Update output files (.xlsx and .json).
</commit_message>
<xml_diff>
--- a/schedules/schedule_classes.xlsx
+++ b/schedules/schedule_classes.xlsx
@@ -987,7 +987,7 @@
       </c>
       <c r="D4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" s="13" t="inlineStr">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="L4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M4" s="13" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="T4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U4" s="13" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="D5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E5" s="15" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="15" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="L5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M5" s="15" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="T5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U5" s="15" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" s="13" t="inlineStr">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="H6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I6" s="13" t="inlineStr">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="L6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M6" s="13" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="P6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="13" t="inlineStr">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="T6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U6" s="13" t="inlineStr">
@@ -1299,7 +1299,7 @@
       </c>
       <c r="D7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="15" t="inlineStr">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="H7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="15" t="inlineStr">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="L7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M7" s="15" t="inlineStr">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="P7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" s="15" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="T7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="15" t="inlineStr">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="13" t="inlineStr">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="H8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I8" s="13" t="inlineStr">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="L8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M8" s="13" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="P8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q8" s="13" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="T8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U8" s="13" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="D9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="15" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="H9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I9" s="15" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="L9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M9" s="15" t="inlineStr">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="P9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q9" s="15" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="T9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U9" s="15" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="D10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E10" s="13" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="H10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I10" s="13" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="L10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M10" s="13" t="inlineStr">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="P10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q10" s="13" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="T10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U10" s="13" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E11" s="15" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="H11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I11" s="15" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="L11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M11" s="15" t="inlineStr">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="P11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q11" s="15" t="inlineStr">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="T11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U11" s="15" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D12" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E12" s="18" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="P12" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q12" s="18" t="inlineStr">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="T4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U4" s="13" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="15" t="inlineStr">
@@ -2259,7 +2259,7 @@
       </c>
       <c r="T5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U5" s="15" t="inlineStr">
@@ -2287,7 +2287,7 @@
       </c>
       <c r="D6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" s="13" t="inlineStr">
@@ -2305,7 +2305,7 @@
       </c>
       <c r="H6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I6" s="13" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="P6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="13" t="inlineStr">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="T6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U6" s="13" t="inlineStr">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="15" t="inlineStr">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="H7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="15" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="P7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" s="15" t="inlineStr">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="T7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="15" t="inlineStr">
@@ -2507,7 +2507,7 @@
       </c>
       <c r="H8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I8" s="13" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="P8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q8" s="13" t="inlineStr">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="T8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U8" s="13" t="inlineStr">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="H10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I10" s="15" t="inlineStr">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="T10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U10" s="15" t="inlineStr">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="H12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I12" s="13" t="inlineStr">
@@ -2795,7 +2795,7 @@
       </c>
       <c r="T12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U12" s="13" t="inlineStr">
@@ -3235,7 +3235,7 @@
       </c>
       <c r="D4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" s="13" t="inlineStr">
@@ -3253,7 +3253,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="D6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" s="15" t="inlineStr">
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="15" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="13" t="inlineStr">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="L8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M8" s="13" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="D10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E10" s="15" t="inlineStr">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="L10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M10" s="15" t="inlineStr">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="P10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q10" s="15" t="inlineStr">
@@ -3895,7 +3895,7 @@
       </c>
       <c r="D12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E12" s="13" t="inlineStr">
@@ -3931,7 +3931,7 @@
       </c>
       <c r="L12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M12" s="13" t="inlineStr">
@@ -3951,7 +3951,7 @@
       </c>
       <c r="P12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q12" s="13" t="inlineStr">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="T12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U12" s="13" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="D14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E14" s="15" t="inlineStr">
@@ -4075,7 +4075,7 @@
       </c>
       <c r="L14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M14" s="15" t="inlineStr">
@@ -4095,7 +4095,7 @@
       </c>
       <c r="P14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q14" s="15" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="T14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U14" s="15" t="inlineStr">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E16" s="13" t="inlineStr">
@@ -4219,7 +4219,7 @@
       </c>
       <c r="L16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M16" s="13" t="inlineStr">
@@ -4237,7 +4237,7 @@
       </c>
       <c r="P16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q16" s="13" t="inlineStr">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="T16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U16" s="13" t="inlineStr">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="D17" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E17" s="15" t="inlineStr">
@@ -4309,7 +4309,7 @@
       </c>
       <c r="P17" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q17" s="15" t="inlineStr">
@@ -4327,7 +4327,7 @@
       </c>
       <c r="T17" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U17" s="15" t="inlineStr">
@@ -4355,7 +4355,7 @@
       </c>
       <c r="D18" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E18" s="18" t="inlineStr">
@@ -4383,7 +4383,7 @@
       </c>
       <c r="P18" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q18" s="18" t="inlineStr">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="T18" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U18" s="18" t="inlineStr">
@@ -4667,7 +4667,7 @@
       </c>
       <c r="D4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" s="13" t="inlineStr">
@@ -4813,7 +4813,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -4831,7 +4831,7 @@
       </c>
       <c r="T5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U5" s="15" t="inlineStr">
@@ -4935,7 +4935,7 @@
       </c>
       <c r="H7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="13" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="L7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M7" s="13" t="inlineStr">
@@ -4989,7 +4989,7 @@
       </c>
       <c r="T7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="13" t="inlineStr">
@@ -5059,7 +5059,7 @@
       </c>
       <c r="D9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="15" t="inlineStr">
@@ -5077,7 +5077,7 @@
       </c>
       <c r="H9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I9" s="15" t="inlineStr">
@@ -5095,7 +5095,7 @@
       </c>
       <c r="L9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M9" s="15" t="inlineStr">
@@ -5131,7 +5131,7 @@
       </c>
       <c r="T9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U9" s="15" t="inlineStr">
@@ -5201,7 +5201,7 @@
       </c>
       <c r="D11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E11" s="13" t="inlineStr">
@@ -5219,7 +5219,7 @@
       </c>
       <c r="H11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I11" s="13" t="inlineStr">
@@ -5237,7 +5237,7 @@
       </c>
       <c r="L11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M11" s="13" t="inlineStr">
@@ -5273,7 +5273,7 @@
       </c>
       <c r="T11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U11" s="13" t="inlineStr">
@@ -5345,7 +5345,7 @@
       </c>
       <c r="D13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E13" s="15" t="inlineStr">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="H13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I13" s="15" t="inlineStr">
@@ -5383,7 +5383,7 @@
       </c>
       <c r="L13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M13" s="15" t="inlineStr">
@@ -5419,7 +5419,7 @@
       </c>
       <c r="T13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U13" s="15" t="inlineStr">
@@ -5491,7 +5491,7 @@
       </c>
       <c r="D15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E15" s="13" t="inlineStr">
@@ -5509,7 +5509,7 @@
       </c>
       <c r="H15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I15" s="13" t="inlineStr">
@@ -5527,7 +5527,7 @@
       </c>
       <c r="L15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M15" s="13" t="inlineStr">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="P15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q15" s="13" t="inlineStr">
@@ -5563,7 +5563,7 @@
       </c>
       <c r="T15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U15" s="13" t="inlineStr">
@@ -5591,7 +5591,7 @@
       </c>
       <c r="D16" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E16" s="15" t="inlineStr">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="H16" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I16" s="15" t="inlineStr">
@@ -5627,7 +5627,7 @@
       </c>
       <c r="L16" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M16" s="15" t="inlineStr">
@@ -5645,7 +5645,7 @@
       </c>
       <c r="P16" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q16" s="15" t="inlineStr">
@@ -5677,7 +5677,7 @@
       </c>
       <c r="D17" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E17" s="18" t="inlineStr">
@@ -5962,7 +5962,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -5980,7 +5980,7 @@
       </c>
       <c r="L4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M4" s="13" t="inlineStr">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="D6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" s="15" t="inlineStr">
@@ -6106,7 +6106,7 @@
       </c>
       <c r="H6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I6" s="15" t="inlineStr">
@@ -6124,7 +6124,7 @@
       </c>
       <c r="L6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M6" s="15" t="inlineStr">
@@ -6142,7 +6142,7 @@
       </c>
       <c r="P6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="15" t="inlineStr">
@@ -6232,7 +6232,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="13" t="inlineStr">
@@ -6250,7 +6250,7 @@
       </c>
       <c r="H8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I8" s="13" t="inlineStr">
@@ -6268,7 +6268,7 @@
       </c>
       <c r="L8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M8" s="13" t="inlineStr">
@@ -6286,7 +6286,7 @@
       </c>
       <c r="P8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q8" s="13" t="inlineStr">
@@ -6306,7 +6306,7 @@
       </c>
       <c r="T8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U8" s="13" t="inlineStr">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="D9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="15" t="inlineStr">
@@ -6352,7 +6352,7 @@
       </c>
       <c r="H9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I9" s="15" t="inlineStr">
@@ -6372,7 +6372,7 @@
       </c>
       <c r="L9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M9" s="15" t="inlineStr">
@@ -6390,7 +6390,7 @@
       </c>
       <c r="P9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q9" s="15" t="inlineStr">
@@ -6408,7 +6408,7 @@
       </c>
       <c r="T9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U9" s="15" t="inlineStr">
@@ -6436,7 +6436,7 @@
       </c>
       <c r="D10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E10" s="13" t="inlineStr">
@@ -6456,7 +6456,7 @@
       </c>
       <c r="H10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I10" s="13" t="inlineStr">
@@ -6474,7 +6474,7 @@
       </c>
       <c r="L10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M10" s="13" t="inlineStr">
@@ -6492,7 +6492,7 @@
       </c>
       <c r="P10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q10" s="13" t="inlineStr">
@@ -6510,7 +6510,7 @@
       </c>
       <c r="T10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U10" s="13" t="inlineStr">
@@ -6538,7 +6538,7 @@
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E11" s="15" t="inlineStr">
@@ -6596,7 +6596,7 @@
       </c>
       <c r="P11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q11" s="15" t="inlineStr">
@@ -6614,7 +6614,7 @@
       </c>
       <c r="T11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U11" s="15" t="inlineStr">
@@ -6756,7 +6756,7 @@
       </c>
       <c r="P13" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q13" s="13" t="inlineStr">
@@ -6774,7 +6774,7 @@
       </c>
       <c r="T13" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U13" s="13" t="inlineStr">
@@ -6928,7 +6928,7 @@
       </c>
       <c r="P15" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q15" s="15" t="inlineStr">
@@ -6946,7 +6946,7 @@
       </c>
       <c r="T15" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U15" s="15" t="inlineStr">
@@ -7050,7 +7050,7 @@
       </c>
       <c r="H17" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I17" s="18" t="inlineStr">
@@ -7403,7 +7403,7 @@
       </c>
       <c r="T4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U4" s="13" t="inlineStr">
@@ -7591,7 +7591,7 @@
       </c>
       <c r="T6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U6" s="15" t="inlineStr">
@@ -7781,7 +7781,7 @@
       </c>
       <c r="T8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U8" s="13" t="inlineStr">
@@ -7919,7 +7919,7 @@
       </c>
       <c r="H10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I10" s="15" t="inlineStr">
@@ -7973,7 +7973,7 @@
       </c>
       <c r="T10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U10" s="15" t="inlineStr">
@@ -8095,7 +8095,7 @@
       </c>
       <c r="H12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I12" s="13" t="inlineStr">
@@ -8113,7 +8113,7 @@
       </c>
       <c r="L12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M12" s="13" t="inlineStr">
@@ -8131,7 +8131,7 @@
       </c>
       <c r="P12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q12" s="13" t="inlineStr">
@@ -8149,7 +8149,7 @@
       </c>
       <c r="T12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U12" s="13" t="inlineStr">
@@ -8241,7 +8241,7 @@
       </c>
       <c r="H14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I14" s="15" t="inlineStr">
@@ -8259,7 +8259,7 @@
       </c>
       <c r="L14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M14" s="15" t="inlineStr">
@@ -8277,7 +8277,7 @@
       </c>
       <c r="P14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q14" s="15" t="inlineStr">
@@ -8295,7 +8295,7 @@
       </c>
       <c r="T14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U14" s="15" t="inlineStr">
@@ -8367,7 +8367,7 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E16" s="13" t="inlineStr">
@@ -8403,7 +8403,7 @@
       </c>
       <c r="L16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M16" s="13" t="inlineStr">
@@ -8421,7 +8421,7 @@
       </c>
       <c r="P16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q16" s="13" t="inlineStr">
@@ -8439,7 +8439,7 @@
       </c>
       <c r="T16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U16" s="13" t="inlineStr">
@@ -8511,7 +8511,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E18" s="15" t="inlineStr">
@@ -8533,7 +8533,7 @@
       </c>
       <c r="L18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M18" s="15" t="inlineStr">
@@ -8577,7 +8577,7 @@
       </c>
       <c r="L19" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M19" s="18" t="inlineStr">
@@ -8872,7 +8872,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -8946,7 +8946,7 @@
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="15" t="inlineStr">
@@ -9076,7 +9076,7 @@
       </c>
       <c r="H7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="13" t="inlineStr">
@@ -9190,7 +9190,7 @@
       </c>
       <c r="D9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="15" t="inlineStr">
@@ -9208,7 +9208,7 @@
       </c>
       <c r="H9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I9" s="15" t="inlineStr">
@@ -9306,7 +9306,7 @@
       </c>
       <c r="D11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E11" s="13" t="inlineStr">
@@ -9324,7 +9324,7 @@
       </c>
       <c r="H11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I11" s="13" t="inlineStr">
@@ -9342,7 +9342,7 @@
       </c>
       <c r="L11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M11" s="13" t="inlineStr">
@@ -9378,7 +9378,7 @@
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E12" s="15" t="inlineStr">
@@ -9396,7 +9396,7 @@
       </c>
       <c r="H12" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I12" s="15" t="inlineStr">
@@ -9414,7 +9414,7 @@
       </c>
       <c r="L12" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M12" s="15" t="inlineStr">
@@ -9450,7 +9450,7 @@
       </c>
       <c r="D13" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E13" s="18" t="inlineStr">
@@ -9472,7 +9472,7 @@
       </c>
       <c r="L13" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M13" s="18" t="inlineStr">
@@ -9755,7 +9755,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -9773,7 +9773,7 @@
       </c>
       <c r="T4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U4" s="13" t="inlineStr">
@@ -9813,7 +9813,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -9871,7 +9871,7 @@
       </c>
       <c r="P6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="13" t="inlineStr">
@@ -10051,7 +10051,7 @@
       </c>
       <c r="T9" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U9" s="13" t="inlineStr">
@@ -10237,7 +10237,7 @@
       </c>
       <c r="P13" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q13" s="13" t="inlineStr">
@@ -10667,7 +10667,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -10727,7 +10727,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -10787,7 +10787,7 @@
       </c>
       <c r="P6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="13" t="inlineStr">
@@ -10805,7 +10805,7 @@
       </c>
       <c r="T6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U6" s="13" t="inlineStr">
@@ -10865,7 +10865,7 @@
       </c>
       <c r="T7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="15" t="inlineStr">
@@ -10965,7 +10965,7 @@
       </c>
       <c r="T9" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U9" s="13" t="inlineStr">
@@ -11049,7 +11049,7 @@
       </c>
       <c r="P11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q11" s="15" t="inlineStr">
@@ -11109,7 +11109,7 @@
       </c>
       <c r="P12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q12" s="13" t="inlineStr">
@@ -11169,7 +11169,7 @@
       </c>
       <c r="P13" s="20" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q13" s="20" t="inlineStr">
@@ -11513,7 +11513,7 @@
       </c>
       <c r="T5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U5" s="15" t="inlineStr">
@@ -11553,7 +11553,7 @@
       </c>
       <c r="P6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="13" t="inlineStr">
@@ -11571,7 +11571,7 @@
       </c>
       <c r="T6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U6" s="13" t="inlineStr">
@@ -11611,7 +11611,7 @@
       </c>
       <c r="P7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" s="15" t="inlineStr">
@@ -11629,7 +11629,7 @@
       </c>
       <c r="T7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="15" t="inlineStr">
@@ -11669,7 +11669,7 @@
       </c>
       <c r="P8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q8" s="13" t="inlineStr">
@@ -11687,7 +11687,7 @@
       </c>
       <c r="T8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U8" s="13" t="inlineStr">
@@ -11727,7 +11727,7 @@
       </c>
       <c r="P9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q9" s="15" t="inlineStr">
@@ -11849,7 +11849,7 @@
       </c>
       <c r="T11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U11" s="13" t="inlineStr">
@@ -12219,7 +12219,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -12237,7 +12237,7 @@
       </c>
       <c r="L4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M4" s="13" t="inlineStr">
@@ -12255,7 +12255,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -12293,7 +12293,7 @@
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="15" t="inlineStr">
@@ -12313,7 +12313,7 @@
       </c>
       <c r="L5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M5" s="15" t="inlineStr">
@@ -12331,7 +12331,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -12365,7 +12365,7 @@
       </c>
       <c r="D6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" s="13" t="inlineStr">
@@ -12383,7 +12383,7 @@
       </c>
       <c r="H6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I6" s="13" t="inlineStr">
@@ -12425,7 +12425,7 @@
       </c>
       <c r="D7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="15" t="inlineStr">
@@ -12451,7 +12451,7 @@
       </c>
       <c r="P7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" s="15" t="inlineStr">
@@ -12469,7 +12469,7 @@
       </c>
       <c r="T7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="15" t="inlineStr">
@@ -12497,7 +12497,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="13" t="inlineStr">
@@ -12639,7 +12639,7 @@
       </c>
       <c r="L12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M12" s="13" t="inlineStr">
@@ -12657,7 +12657,7 @@
       </c>
       <c r="P12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q12" s="13" t="inlineStr">
@@ -12701,7 +12701,7 @@
       </c>
       <c r="P13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q13" s="15" t="inlineStr">
@@ -12719,7 +12719,7 @@
       </c>
       <c r="T13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U13" s="15" t="inlineStr">
@@ -12781,7 +12781,7 @@
       </c>
       <c r="H15" s="20" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I15" s="20" t="inlineStr">
@@ -13297,7 +13297,7 @@
       </c>
       <c r="L6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M6" s="15" t="inlineStr">
@@ -13671,7 +13671,7 @@
       </c>
       <c r="H10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I10" s="15" t="inlineStr">
@@ -13725,7 +13725,7 @@
       </c>
       <c r="T10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U10" s="15" t="inlineStr">
@@ -13845,7 +13845,7 @@
       </c>
       <c r="H12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I12" s="13" t="inlineStr">
@@ -13899,7 +13899,7 @@
       </c>
       <c r="T12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U12" s="13" t="inlineStr">
@@ -14015,7 +14015,7 @@
       </c>
       <c r="H14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I14" s="15" t="inlineStr">
@@ -14033,7 +14033,7 @@
       </c>
       <c r="L14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M14" s="15" t="inlineStr">
@@ -14071,7 +14071,7 @@
       </c>
       <c r="T14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U14" s="15" t="inlineStr">
@@ -14175,7 +14175,7 @@
       </c>
       <c r="H16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I16" s="13" t="inlineStr">
@@ -14193,7 +14193,7 @@
       </c>
       <c r="L16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M16" s="13" t="inlineStr">
@@ -14211,7 +14211,7 @@
       </c>
       <c r="P16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q16" s="13" t="inlineStr">
@@ -14229,7 +14229,7 @@
       </c>
       <c r="T16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U16" s="13" t="inlineStr">
@@ -14321,7 +14321,7 @@
       </c>
       <c r="H18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I18" s="15" t="inlineStr">
@@ -14339,7 +14339,7 @@
       </c>
       <c r="L18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M18" s="15" t="inlineStr">
@@ -14357,7 +14357,7 @@
       </c>
       <c r="P18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q18" s="15" t="inlineStr">
@@ -14485,7 +14485,7 @@
       </c>
       <c r="L20" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M20" s="13" t="inlineStr">
@@ -14843,7 +14843,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -14887,7 +14887,7 @@
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="15" t="inlineStr">
@@ -14957,7 +14957,7 @@
       </c>
       <c r="D7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="15" t="inlineStr">
@@ -14975,7 +14975,7 @@
       </c>
       <c r="H7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="15" t="inlineStr">
@@ -14997,7 +14997,7 @@
       </c>
       <c r="P7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" s="15" t="inlineStr">
@@ -15041,7 +15041,7 @@
       </c>
       <c r="P8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q8" s="13" t="inlineStr">
@@ -15081,7 +15081,7 @@
       </c>
       <c r="L9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M9" s="15" t="inlineStr">
@@ -15159,7 +15159,7 @@
       </c>
       <c r="P11" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q11" s="15" t="inlineStr">
@@ -15195,7 +15195,7 @@
       </c>
       <c r="H12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I12" s="13" t="inlineStr">
@@ -15241,7 +15241,7 @@
       </c>
       <c r="H13" s="20" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I13" s="20" t="inlineStr">
@@ -15261,7 +15261,7 @@
       </c>
       <c r="L13" s="20" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M13" s="20" t="inlineStr">
@@ -15571,7 +15571,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -15611,7 +15611,7 @@
       </c>
       <c r="L6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M6" s="13" t="inlineStr">
@@ -15629,7 +15629,7 @@
       </c>
       <c r="P6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="13" t="inlineStr">
@@ -15647,7 +15647,7 @@
       </c>
       <c r="T6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U6" s="13" t="inlineStr">
@@ -15675,7 +15675,7 @@
       </c>
       <c r="D7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="15" t="inlineStr">
@@ -15697,7 +15697,7 @@
       </c>
       <c r="L7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M7" s="15" t="inlineStr">
@@ -15715,7 +15715,7 @@
       </c>
       <c r="P7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" s="15" t="inlineStr">
@@ -15733,7 +15733,7 @@
       </c>
       <c r="T7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="15" t="inlineStr">
@@ -15765,7 +15765,7 @@
       </c>
       <c r="H8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I8" s="13" t="inlineStr">
@@ -15783,7 +15783,7 @@
       </c>
       <c r="L8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M8" s="13" t="inlineStr">
@@ -15801,7 +15801,7 @@
       </c>
       <c r="P8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q8" s="13" t="inlineStr">
@@ -15819,7 +15819,7 @@
       </c>
       <c r="T8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U8" s="13" t="inlineStr">
@@ -15847,7 +15847,7 @@
       </c>
       <c r="D9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="15" t="inlineStr">
@@ -15873,7 +15873,7 @@
       </c>
       <c r="P9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q9" s="15" t="inlineStr">
@@ -15905,7 +15905,7 @@
       </c>
       <c r="D10" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E10" s="18" t="inlineStr">
@@ -16185,7 +16185,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -16203,7 +16203,7 @@
       </c>
       <c r="L4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M4" s="13" t="inlineStr">
@@ -16243,7 +16243,7 @@
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="15" t="inlineStr">
@@ -16261,7 +16261,7 @@
       </c>
       <c r="L5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M5" s="15" t="inlineStr">
@@ -16305,7 +16305,7 @@
       </c>
       <c r="L6" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M6" s="13" t="inlineStr">
@@ -16345,7 +16345,7 @@
       </c>
       <c r="H7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="15" t="inlineStr">
@@ -16363,7 +16363,7 @@
       </c>
       <c r="L7" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M7" s="15" t="inlineStr">
@@ -16399,7 +16399,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="13" t="inlineStr">
@@ -16443,7 +16443,7 @@
       </c>
       <c r="D9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="15" t="inlineStr">
@@ -16495,7 +16495,7 @@
       </c>
       <c r="L10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M10" s="13" t="inlineStr">
@@ -16561,7 +16561,7 @@
       </c>
       <c r="D12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E12" s="13" t="inlineStr">
@@ -16605,7 +16605,7 @@
       </c>
       <c r="D13" s="20" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E13" s="20" t="inlineStr">
@@ -16881,7 +16881,7 @@
       </c>
       <c r="D4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" s="13" t="inlineStr">
@@ -16899,7 +16899,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -16917,7 +16917,7 @@
       </c>
       <c r="L4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M4" s="13" t="inlineStr">
@@ -16935,7 +16935,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -16983,7 +16983,7 @@
       </c>
       <c r="D5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E5" s="15" t="inlineStr">
@@ -17003,7 +17003,7 @@
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="15" t="inlineStr">
@@ -17023,7 +17023,7 @@
       </c>
       <c r="L5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M5" s="15" t="inlineStr">
@@ -17041,7 +17041,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -17131,7 +17131,7 @@
       </c>
       <c r="D7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="13" t="inlineStr">
@@ -17149,7 +17149,7 @@
       </c>
       <c r="H7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="13" t="inlineStr">
@@ -17187,7 +17187,7 @@
       </c>
       <c r="P7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" s="13" t="inlineStr">
@@ -17289,7 +17289,7 @@
       </c>
       <c r="D9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="15" t="inlineStr">
@@ -17325,7 +17325,7 @@
       </c>
       <c r="L9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M9" s="15" t="inlineStr">
@@ -17343,7 +17343,7 @@
       </c>
       <c r="P9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q9" s="15" t="inlineStr">
@@ -17361,7 +17361,7 @@
       </c>
       <c r="T9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U9" s="15" t="inlineStr">
@@ -17431,7 +17431,7 @@
       </c>
       <c r="D11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E11" s="13" t="inlineStr">
@@ -17485,7 +17485,7 @@
       </c>
       <c r="P11" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q11" s="13" t="inlineStr">
@@ -17649,7 +17649,7 @@
       </c>
       <c r="D14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E14" s="15" t="inlineStr">
@@ -17703,7 +17703,7 @@
       </c>
       <c r="P14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q14" s="15" t="inlineStr">
@@ -17867,7 +17867,7 @@
       </c>
       <c r="D17" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E17" s="13" t="inlineStr">
@@ -18087,7 +18087,7 @@
       </c>
       <c r="D20" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E20" s="15" t="inlineStr">
@@ -18303,7 +18303,7 @@
       </c>
       <c r="P23" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q23" s="13" t="inlineStr">
@@ -18619,7 +18619,7 @@
       </c>
       <c r="D4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" s="13" t="inlineStr">
@@ -18637,7 +18637,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -18673,7 +18673,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -18691,7 +18691,7 @@
       </c>
       <c r="T4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U4" s="13" t="inlineStr">
@@ -18719,7 +18719,7 @@
       </c>
       <c r="D5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E5" s="15" t="inlineStr">
@@ -18737,7 +18737,7 @@
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" s="15" t="inlineStr">
@@ -18773,7 +18773,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -18791,7 +18791,7 @@
       </c>
       <c r="T5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U5" s="15" t="inlineStr">
@@ -18861,7 +18861,7 @@
       </c>
       <c r="D7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="13" t="inlineStr">
@@ -18879,7 +18879,7 @@
       </c>
       <c r="H7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I7" s="13" t="inlineStr">
@@ -19051,7 +19051,7 @@
       </c>
       <c r="H9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I9" s="15" t="inlineStr">
@@ -19465,7 +19465,7 @@
       </c>
       <c r="L13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M13" s="15" t="inlineStr">
@@ -19503,7 +19503,7 @@
       </c>
       <c r="T13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U13" s="15" t="inlineStr">
@@ -19603,7 +19603,7 @@
       </c>
       <c r="D15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E15" s="13" t="inlineStr">
@@ -19657,7 +19657,7 @@
       </c>
       <c r="P15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q15" s="13" t="inlineStr">
@@ -19675,7 +19675,7 @@
       </c>
       <c r="T15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U15" s="13" t="inlineStr">
@@ -19745,7 +19745,7 @@
       </c>
       <c r="D17" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E17" s="15" t="inlineStr">
@@ -19803,7 +19803,7 @@
       </c>
       <c r="T17" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U17" s="15" t="inlineStr">
@@ -20184,7 +20184,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -20202,7 +20202,7 @@
       </c>
       <c r="T4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U4" s="13" t="inlineStr">
@@ -20230,7 +20230,7 @@
       </c>
       <c r="D5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E5" s="15" t="inlineStr">
@@ -20288,7 +20288,7 @@
       </c>
       <c r="P5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" s="15" t="inlineStr">
@@ -20306,7 +20306,7 @@
       </c>
       <c r="T5" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U5" s="15" t="inlineStr">
@@ -20376,7 +20376,7 @@
       </c>
       <c r="D7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E7" s="13" t="inlineStr">
@@ -20414,7 +20414,7 @@
       </c>
       <c r="L7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M7" s="13" t="inlineStr">
@@ -20432,7 +20432,7 @@
       </c>
       <c r="P7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q7" s="13" t="inlineStr">
@@ -20450,7 +20450,7 @@
       </c>
       <c r="T7" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U7" s="13" t="inlineStr">
@@ -20520,7 +20520,7 @@
       </c>
       <c r="D9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" s="15" t="inlineStr">
@@ -20538,7 +20538,7 @@
       </c>
       <c r="H9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I9" s="15" t="inlineStr">
@@ -20556,7 +20556,7 @@
       </c>
       <c r="L9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M9" s="15" t="inlineStr">
@@ -20574,7 +20574,7 @@
       </c>
       <c r="P9" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q9" s="15" t="inlineStr">
@@ -20620,7 +20620,7 @@
       </c>
       <c r="D10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E10" s="13" t="inlineStr">
@@ -20656,7 +20656,7 @@
       </c>
       <c r="L10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M10" s="13" t="inlineStr">
@@ -20674,7 +20674,7 @@
       </c>
       <c r="P10" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q10" s="13" t="inlineStr">
@@ -20800,7 +20800,7 @@
       </c>
       <c r="L12" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M12" s="15" t="inlineStr">
@@ -20918,7 +20918,7 @@
       </c>
       <c r="L14" s="18" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M14" s="18" t="inlineStr">
@@ -21206,7 +21206,7 @@
       </c>
       <c r="D4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" s="13" t="inlineStr">
@@ -21224,7 +21224,7 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I4" s="13" t="inlineStr">
@@ -21242,7 +21242,7 @@
       </c>
       <c r="L4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M4" s="13" t="inlineStr">
@@ -21278,7 +21278,7 @@
       </c>
       <c r="T4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U4" s="13" t="inlineStr">
@@ -21348,7 +21348,7 @@
       </c>
       <c r="D6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" s="15" t="inlineStr">
@@ -21366,7 +21366,7 @@
       </c>
       <c r="H6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I6" s="15" t="inlineStr">
@@ -21384,7 +21384,7 @@
       </c>
       <c r="L6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M6" s="15" t="inlineStr">
@@ -21420,7 +21420,7 @@
       </c>
       <c r="T6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U6" s="15" t="inlineStr">
@@ -21490,7 +21490,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="13" t="inlineStr">
@@ -21508,7 +21508,7 @@
       </c>
       <c r="H8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I8" s="13" t="inlineStr">
@@ -21562,7 +21562,7 @@
       </c>
       <c r="T8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U8" s="13" t="inlineStr">
@@ -21666,7 +21666,7 @@
       </c>
       <c r="H10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I10" s="15" t="inlineStr">
@@ -21722,7 +21722,7 @@
       </c>
       <c r="T10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U10" s="15" t="inlineStr">
@@ -22102,7 +22102,7 @@
       </c>
       <c r="T14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U14" s="15" t="inlineStr">
@@ -22222,7 +22222,7 @@
       </c>
       <c r="H16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I16" s="13" t="inlineStr">
@@ -22402,7 +22402,7 @@
       </c>
       <c r="H18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I18" s="15" t="inlineStr">
@@ -22460,7 +22460,7 @@
       </c>
       <c r="T18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U18" s="15" t="inlineStr">
@@ -23130,7 +23130,7 @@
       </c>
       <c r="P8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q8" s="13" t="inlineStr">
@@ -23148,7 +23148,7 @@
       </c>
       <c r="T8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U8" s="13" t="inlineStr">
@@ -23292,7 +23292,7 @@
       </c>
       <c r="P10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q10" s="15" t="inlineStr">
@@ -23310,7 +23310,7 @@
       </c>
       <c r="T10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U10" s="15" t="inlineStr">
@@ -23398,7 +23398,7 @@
       </c>
       <c r="D12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E12" s="13" t="inlineStr">
@@ -23416,7 +23416,7 @@
       </c>
       <c r="H12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I12" s="13" t="inlineStr">
@@ -23434,7 +23434,7 @@
       </c>
       <c r="L12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M12" s="13" t="inlineStr">
@@ -23452,7 +23452,7 @@
       </c>
       <c r="P12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q12" s="13" t="inlineStr">
@@ -23470,7 +23470,7 @@
       </c>
       <c r="T12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U12" s="13" t="inlineStr">
@@ -23518,7 +23518,7 @@
       </c>
       <c r="H13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I13" s="15" t="inlineStr">
@@ -23536,7 +23536,7 @@
       </c>
       <c r="L13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M13" s="15" t="inlineStr">
@@ -23554,7 +23554,7 @@
       </c>
       <c r="P13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q13" s="15" t="inlineStr">
@@ -23572,7 +23572,7 @@
       </c>
       <c r="T13" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U13" s="15" t="inlineStr">
@@ -23642,7 +23642,7 @@
       </c>
       <c r="D15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E15" s="13" t="inlineStr">
@@ -23660,7 +23660,7 @@
       </c>
       <c r="H15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I15" s="13" t="inlineStr">
@@ -23678,7 +23678,7 @@
       </c>
       <c r="L15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M15" s="13" t="inlineStr">
@@ -23696,7 +23696,7 @@
       </c>
       <c r="P15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q15" s="13" t="inlineStr">
@@ -23714,7 +23714,7 @@
       </c>
       <c r="T15" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U15" s="13" t="inlineStr">
@@ -23760,7 +23760,7 @@
       </c>
       <c r="H16" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I16" s="15" t="inlineStr">
@@ -23778,7 +23778,7 @@
       </c>
       <c r="L16" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M16" s="15" t="inlineStr">
@@ -23796,7 +23796,7 @@
       </c>
       <c r="P16" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q16" s="15" t="inlineStr">
@@ -23814,7 +23814,7 @@
       </c>
       <c r="T16" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U16" s="15" t="inlineStr">
@@ -23904,7 +23904,7 @@
       </c>
       <c r="H18" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I18" s="13" t="inlineStr">
@@ -23962,7 +23962,7 @@
       </c>
       <c r="T18" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U18" s="13" t="inlineStr">
@@ -24552,7 +24552,7 @@
       </c>
       <c r="D4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" s="13" t="inlineStr">
@@ -24574,7 +24574,7 @@
       </c>
       <c r="L4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M4" s="13" t="inlineStr">
@@ -24684,7 +24684,7 @@
       </c>
       <c r="D6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" s="15" t="inlineStr">
@@ -24706,7 +24706,7 @@
       </c>
       <c r="L6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M6" s="15" t="inlineStr">
@@ -24816,7 +24816,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="13" t="inlineStr">
@@ -24854,7 +24854,7 @@
       </c>
       <c r="L8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M8" s="13" t="inlineStr">
@@ -25018,7 +25018,7 @@
       </c>
       <c r="L10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M10" s="15" t="inlineStr">
@@ -25158,7 +25158,7 @@
       </c>
       <c r="D12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E12" s="13" t="inlineStr">
@@ -25176,7 +25176,7 @@
       </c>
       <c r="H12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I12" s="13" t="inlineStr">
@@ -25194,7 +25194,7 @@
       </c>
       <c r="L12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M12" s="13" t="inlineStr">
@@ -25232,7 +25232,7 @@
       </c>
       <c r="T12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U12" s="13" t="inlineStr">
@@ -25320,7 +25320,7 @@
       </c>
       <c r="H14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I14" s="15" t="inlineStr">
@@ -25338,7 +25338,7 @@
       </c>
       <c r="L14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M14" s="15" t="inlineStr">
@@ -25374,7 +25374,7 @@
       </c>
       <c r="T14" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U14" s="15" t="inlineStr">
@@ -25476,7 +25476,7 @@
       </c>
       <c r="H16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I16" s="13" t="inlineStr">
@@ -25494,7 +25494,7 @@
       </c>
       <c r="L16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="M16" s="13" t="inlineStr">
@@ -25530,7 +25530,7 @@
       </c>
       <c r="T16" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U16" s="13" t="inlineStr">
@@ -25616,7 +25616,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E18" s="15" t="inlineStr">
@@ -25634,7 +25634,7 @@
       </c>
       <c r="H18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I18" s="15" t="inlineStr">
@@ -25672,7 +25672,7 @@
       </c>
       <c r="P18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q18" s="15" t="inlineStr">
@@ -25690,7 +25690,7 @@
       </c>
       <c r="T18" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U18" s="15" t="inlineStr">
@@ -25762,7 +25762,7 @@
       </c>
       <c r="D20" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E20" s="13" t="inlineStr">
@@ -26376,7 +26376,7 @@
       </c>
       <c r="P4" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q4" s="13" t="inlineStr">
@@ -26522,7 +26522,7 @@
       </c>
       <c r="P6" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" s="15" t="inlineStr">
@@ -26642,7 +26642,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" s="13" t="inlineStr">
@@ -26838,7 +26838,7 @@
       </c>
       <c r="D10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E10" s="15" t="inlineStr">
@@ -26896,7 +26896,7 @@
       </c>
       <c r="P10" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q10" s="15" t="inlineStr">
@@ -27020,7 +27020,7 @@
       </c>
       <c r="D12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E12" s="13" t="inlineStr">
@@ -27078,7 +27078,7 @@
       </c>
       <c r="P12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q12" s="13" t="inlineStr">
@@ -27096,7 +27096,7 @@
       </c>
       <c r="T12" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U12" s="13" t="inlineStr">
@@ -27300,7 +27300,7 @@
       </c>
       <c r="P15" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q15" s="15" t="inlineStr">
@@ -27318,7 +27318,7 @@
       </c>
       <c r="T15" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U15" s="15" t="inlineStr">
@@ -27478,7 +27478,7 @@
       </c>
       <c r="D18" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E18" s="13" t="inlineStr">
@@ -27536,7 +27536,7 @@
       </c>
       <c r="P18" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q18" s="13" t="inlineStr">
@@ -27554,7 +27554,7 @@
       </c>
       <c r="T18" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U18" s="13" t="inlineStr">
@@ -27640,7 +27640,7 @@
       </c>
       <c r="D20" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E20" s="15" t="inlineStr">
@@ -27698,7 +27698,7 @@
       </c>
       <c r="P20" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q20" s="15" t="inlineStr">
@@ -27716,7 +27716,7 @@
       </c>
       <c r="T20" s="15" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U20" s="15" t="inlineStr">
@@ -27844,7 +27844,7 @@
       </c>
       <c r="P22" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q22" s="13" t="inlineStr">
@@ -27862,7 +27862,7 @@
       </c>
       <c r="T22" s="13" t="inlineStr">
         <is>
-          <t>X</t>
+          <t>-</t>
         </is>
       </c>
       <c r="U22" s="13" t="inlineStr">

</xml_diff>